<commit_message>
Refactored to change the form view and changed the variables
</commit_message>
<xml_diff>
--- a/client/public/AssetBulkUpload.xlsx
+++ b/client/public/AssetBulkUpload.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24411"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F615FA4-FE29-45E9-A652-BF0C9225B84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{61903B48-4B4D-4DFE-99AD-6B94806BBAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,14 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>assetId</t>
   </si>
   <si>
-    <t>assetName</t>
-  </si>
-  <si>
     <t>assetType</t>
   </si>
   <si>
@@ -43,30 +40,30 @@
     <t>invoiceNumber</t>
   </si>
   <si>
-    <t>lastauditDate</t>
-  </si>
-  <si>
-    <t>onboardDate</t>
-  </si>
-  <si>
-    <t>productSerial</t>
+    <t>putToUseDate</t>
+  </si>
+  <si>
+    <t>invoiceDate</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>purchaseOrderDate</t>
+  </si>
+  <si>
+    <t>purchaseOrder</t>
+  </si>
+  <si>
+    <t>vendor</t>
+  </si>
+  <si>
+    <t>location</t>
   </si>
   <si>
     <t>purchaseDate</t>
   </si>
   <si>
-    <t>purchaseOrder</t>
-  </si>
-  <si>
-    <t>vendor</t>
-  </si>
-  <si>
-    <t>warranty</t>
-  </si>
-  <si>
-    <t>warrantyExp</t>
-  </si>
-  <si>
     <t>shelflife</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
   </si>
   <si>
     <t>depmethod</t>
-  </si>
-  <si>
-    <t>Computer New</t>
   </si>
   <si>
     <t>rented</t>
@@ -435,24 +429,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -498,212 +493,206 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>12345</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>15.99</v>
       </c>
       <c r="D2">
-        <v>15.99</v>
-      </c>
-      <c r="E2">
         <v>12345</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44378</v>
       </c>
       <c r="F2" s="1">
         <v>44378</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2">
+        <v>764474</v>
+      </c>
+      <c r="H2" s="1">
         <v>44378</v>
       </c>
-      <c r="H2">
-        <v>764474</v>
-      </c>
-      <c r="I2" s="1">
+      <c r="I2">
+        <v>342342</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2" s="1">
         <v>44378</v>
       </c>
-      <c r="J2">
-        <v>342342</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2">
-        <v>5</v>
-      </c>
-      <c r="M2" s="1">
-        <v>44378</v>
+      <c r="M2">
+        <v>10</v>
       </c>
       <c r="N2">
-        <v>10</v>
-      </c>
-      <c r="O2">
         <v>9.99</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:15">
+      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="H3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="H4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="H5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="H6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="H7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="H8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="H9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="H10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="H11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="H12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="H13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="H14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="H15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="6:13">
+      <c r="H16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="5:12">
+      <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="6:13">
+      <c r="H17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="5:12">
+      <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="6:13">
+      <c r="H18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="5:12">
+      <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="6:13">
+      <c r="H19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="5:12">
+      <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="6:13">
+      <c r="H20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="5:12">
+      <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="6:13">
+      <c r="H21" s="1"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="5:12">
+      <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="6:13">
+      <c r="H22" s="1"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="5:12">
+      <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="6:13">
+      <c r="H23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="5:12">
+      <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="6:13">
+      <c r="H24" s="1"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="5:12">
+      <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="6:13">
+      <c r="H25" s="1"/>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="5:12">
+      <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="6:13">
+      <c r="H26" s="1"/>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="5:12">
+      <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="M27" s="1"/>
-    </row>
-    <row r="28" spans="6:13">
+      <c r="H27" s="1"/>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="5:12">
+      <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="M28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="L28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>